<commit_message>
Termiando el trabajo de Hugo
</commit_message>
<xml_diff>
--- a/Hugo Hernan Henao/Trimestre IV/Evidencias/QuickSort/Documentos/Presupuesto.xlsx
+++ b/Hugo Hernan Henao/Trimestre IV/Evidencias/QuickSort/Documentos/Presupuesto.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructivo" sheetId="2" r:id="rId1"/>
     <sheet name="Datos" sheetId="6" r:id="rId2"/>
     <sheet name="Presupuesto Detallado" sheetId="1" r:id="rId3"/>
-    <sheet name="Por Recursos" sheetId="5" r:id="rId4"/>
+    <sheet name="Por Recursos" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Instructivo!$A$1:$D$34</definedName>
@@ -1388,8 +1388,8 @@
   </sheetPr>
   <dimension ref="B1:J45"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,7 +2188,7 @@
   </sheetPr>
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>